<commit_message>
Add latex but comment out
</commit_message>
<xml_diff>
--- a/references/Reopening_Indicators_Comparison.xlsx
+++ b/references/Reopening_Indicators_Comparison.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\404031\Documents\GitHub\public-health-prototype\notebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\404031\Documents\GitHub\covid19-indicators\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Chicago</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>At least 90 days of PPE stockpiled</t>
-  </si>
-  <si>
-    <t>Capacity to conduct 30 tests per 1,000 residents per month</t>
   </si>
   <si>
     <t>New York State</t>
@@ -151,9 +148,6 @@
     </r>
   </si>
   <si>
-    <t>Test 135,000 per month, equivalent to 4,500 people per day (need to convert to per 1,000 rate per month)</t>
-  </si>
-  <si>
     <t>Stable or declining rates of ICU deaths</t>
   </si>
   <si>
@@ -326,13 +320,218 @@
       <t xml:space="preserve">
 At least 14 days decline in rate of new cases (per capita?) </t>
     </r>
+  </si>
+  <si>
+    <t>California State Indicators</t>
+  </si>
+  <si>
+    <t>Los Angeles County Indicators</t>
+  </si>
+  <si>
+    <t>http://publichealth.lacounty.gov/media/Coronavirus/covid19_recovery_dashboard.htm</t>
+  </si>
+  <si>
+    <t>https://covid19.ca.gov/roadmap-counties/</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <r>
+      <t>Stable hospitalizations of COVID individuals on a 7-day average of daily percent change of less than 5% </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> 
+Fewer than 20 COVID hospitalizations on any single day in the past 14 days </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Less than 25 new cases per 100,000 residents in the past 14 days </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">or 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Less than 8% testing positive in the past 7 days</t>
+    </r>
+  </si>
+  <si>
+    <t>Capacity to conduct 30 tests per 1,000 residents per month. Equivalent to 30 tests per 1,000 residents per month.</t>
+  </si>
+  <si>
+    <t>Test 135,000 per month, equivalent to 4,500 people per day. Equivalent to 50 tests per 1,000 residents per month.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum daily testing volume to test 1.5 per 1,000 residents, which can be met through a combination of testing of symptomatic individuals and targeted surveillance.  The county’s average daily testing volume for the past week must be provided.  If the county does not believe a testing volume of 1.5 per 1,000 residents is merited, justification must be provided. 
+Testing availability for at least 75% of residents, as measured by a specimen collection site (including established health care providers) within 30 minutes driving time in urban areas, and 60 minutes in rural areas. </t>
+  </si>
+  <si>
+    <t>Sufficient contact tracing so public health staff work can work with a patient to help them recall everyone with whom they have had close contact during the timeframe while they may have been infectious.  For counties that have no cases, there should be at least 15 staff per 100,000 county population trained and available for contact tracing; for counties with small populations, there must be at least one staff person trained and available.  </t>
+  </si>
+  <si>
+    <t>County (or regional) hospital capacity to accommodate a minimum surge of 35% due to COVID-19 cases in addition to providing usual care for non-COVID-19 patients. </t>
+  </si>
+  <si>
+    <t>Daily number of deaths, past 7-day average has not increased over past 14 days.
+Attain this even when broken down by race/ethnicity and area poverty.</t>
+  </si>
+  <si>
+    <t>Los Angeles County</t>
+  </si>
+  <si>
+    <t>Daily number of hospitalized COVID-19 patients, past 3-day average has not increased over the past 14 days.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Daily number of available ICU beds, past 3-day average has not decreased over the past 14 days </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+accounts for at least 10% of total ICU bed capacity, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Daily number of available ventilators, past 3-day average has not decreased over the past 14 days </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+accounts for at least 20% of total ventilator capacity, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>At least 60% of hospitals have 15+ days of available PPE, including N95 masks, other masks, eye protection, face shields, gloves, and gowns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 1.5 per 1,000 residents daily. Equivalent to to 45 test per 1,000 residents per month.
+Daily Reported Number of COVID-19 Diagnostic Tests, Past 7 day Average, is 15,000 tests for each day over past 7 days. </t>
+  </si>
+  <si>
+    <t>At least 90% of COVID-19 cases that have follow-up investigation initiated within 1 day of assignment.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,6 +551,28 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -448,7 +669,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -497,6 +718,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -787,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -799,25 +1023,31 @@
     <col min="2" max="2" width="28.54296875" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.7265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="41.08984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="47.90625" style="1" customWidth="1"/>
+    <col min="5" max="7" width="47.90625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -827,8 +1057,10 @@
       <c r="C2" s="6"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="8"/>
       <c r="B3" s="5" t="s">
         <v>4</v>
@@ -836,8 +1068,10 @@
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
@@ -845,53 +1079,69 @@
         <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="10"/>
       <c r="B5" s="17"/>
       <c r="C5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="10"/>
       <c r="B6" s="16"/>
       <c r="C6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="11"/>
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
@@ -899,51 +1149,73 @@
         <v>9</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
       <c r="B9" s="16"/>
       <c r="C9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A10" s="13"/>
       <c r="B10" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A11" s="14"/>
       <c r="B11" s="16"/>
       <c r="C11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -961,54 +1233,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.36328125" customWidth="1"/>
-    <col min="2" max="2" width="59.36328125" customWidth="1"/>
+    <col min="2" max="2" width="63.1796875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1018,6 +1306,8 @@
     <hyperlink ref="B2" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
     <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B6" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>